<commit_message>
SLL part 1 31 Oct 2019
</commit_message>
<xml_diff>
--- a/Daily_plan/2019/10_Oct/29-Oct_01-Nov.xlsx
+++ b/Daily_plan/2019/10_Oct/29-Oct_01-Nov.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="280" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="116">
   <si>
     <t xml:space="preserve">Week_03</t>
   </si>
@@ -51,19 +51,19 @@
     <t xml:space="preserve">Chapter 6  Learn cpp </t>
   </si>
   <si>
-    <t xml:space="preserve">Stack in C and C++</t>
+    <t xml:space="preserve">Stack in C++</t>
   </si>
   <si>
     <t xml:space="preserve">Part 1 completed, Part 2 completed</t>
   </si>
   <si>
-    <t xml:space="preserve">Queue in C and C++</t>
+    <t xml:space="preserve">Queue in C++</t>
   </si>
   <si>
     <t xml:space="preserve">array and loop</t>
   </si>
   <si>
-    <t xml:space="preserve">Linked list in C and C++</t>
+    <t xml:space="preserve">Linked list in C++</t>
   </si>
   <si>
     <t xml:space="preserve">selection sort performed</t>
@@ -74,13 +74,13 @@
 WIP – Work In Progress</t>
   </si>
   <si>
-    <t xml:space="preserve">Double Linked list in C and C++</t>
+    <t xml:space="preserve">Double Linked list in C++</t>
   </si>
   <si>
     <t xml:space="preserve">Multi dimensional array</t>
   </si>
   <si>
-    <t xml:space="preserve">Circular Linked list in C and C++</t>
+    <t xml:space="preserve">Circular Linked list in C++</t>
   </si>
   <si>
     <t xml:space="preserve">C-style string</t>
@@ -167,13 +167,13 @@
     <t xml:space="preserve">pointer to pointer</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Structure: Stack in C and C++</t>
+    <t xml:space="preserve">Data Structure: Stack in C++</t>
   </si>
   <si>
     <t xml:space="preserve">What is data structure, algorithm and stack and implementation of stack</t>
   </si>
   <si>
-    <t xml:space="preserve">Data Structure: Queue in C and C++</t>
+    <t xml:space="preserve">Data Structure: Queue in C++</t>
   </si>
   <si>
     <t xml:space="preserve">Python: OOPs</t>
@@ -200,6 +200,45 @@
     <t xml:space="preserve">30-10-2019</t>
   </si>
   <si>
+    <t xml:space="preserve">Completed the stack in c++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Structure: Queue in  C++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Completed the queue in c++</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Thu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31-10-2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Miscellaneous Activity (Knowledge updation based on CV)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Went through C++ basic, Attended online test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">20-06-2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daily Task                        </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acual Task</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> % Completed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plan Hrs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual Hrs</t>
+  </si>
+  <si>
     <t xml:space="preserve">An introduction to std::array</t>
   </si>
   <si>
@@ -213,42 +252,6 @@
   </si>
   <si>
     <t xml:space="preserve">Data Structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revise Stack with C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revise Queue with C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Stack with C++</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Miscellaneous Activity (Knowledge updation based on CV)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Went through C++ basic, Attended online test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Thu</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-06-2019</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daily Task                        </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Acual Task</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> % Completed</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Plan Hrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actual Hrs</t>
   </si>
   <si>
     <t xml:space="preserve">Queue using linked list using C</t>
@@ -512,14 +515,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF669900"/>
-        <bgColor rgb="FF339966"/>
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF669900"/>
+        <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
   </fills>
@@ -658,14 +661,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -677,8 +672,16 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -689,7 +692,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -794,15 +797,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4897959183674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.1530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.1224489795918"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.6224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.8775510204082"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.71938775510204"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.6785714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -860,7 +862,8 @@
         <v>3</v>
       </c>
       <c r="F4" s="12" t="n">
-        <v>4</v>
+        <f aca="false">4+2</f>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -879,9 +882,12 @@
       <c r="E5" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="12"/>
-    </row>
-    <row r="6" customFormat="false" ht="35.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F5" s="12" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
         <v>3</v>
       </c>
@@ -1073,7 +1079,8 @@
         <v>0.5</v>
       </c>
       <c r="F16" s="12" t="n">
-        <v>0.5</v>
+        <f aca="false">0.5+0.5</f>
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1093,7 +1100,8 @@
         <v>0.5</v>
       </c>
       <c r="F17" s="12" t="n">
-        <v>1</v>
+        <f aca="false">1+1.5</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1184,7 +1192,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="n">
         <v>1</v>
       </c>
@@ -1350,33 +1358,45 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="11"/>
+      <c r="C32" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="E32" s="12" t="n">
         <v>1.5</v>
       </c>
-      <c r="F32" s="12"/>
+      <c r="F32" s="12" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="n">
         <v>2</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="18"/>
+        <v>59</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="E33" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F33" s="19"/>
+      <c r="F33" s="19" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="4" t="n">
@@ -1399,12 +1419,18 @@
       <c r="B35" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="18"/>
+      <c r="C35" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="E35" s="19" t="n">
         <v>0.5</v>
       </c>
-      <c r="F35" s="19"/>
+      <c r="F35" s="19" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="n">
@@ -1413,12 +1439,18 @@
       <c r="B36" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="18"/>
+      <c r="C36" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="E36" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="F36" s="19"/>
+      <c r="F36" s="19" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="4" t="n">
@@ -1451,142 +1483,134 @@
       <c r="F38" s="22"/>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="12" t="n">
-        <v>1</v>
+      <c r="A39" s="4" t="s">
+        <v>61</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C39" s="10" t="s">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D39" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E39" s="12" t="n">
         <v>0.5</v>
       </c>
       <c r="F39" s="12" t="n">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="12" t="n">
-        <v>2</v>
+      <c r="A40" s="4" t="n">
+        <v>19</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C40" s="10" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="D40" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E40" s="12" t="n">
         <v>0.5</v>
       </c>
       <c r="F40" s="12" t="n">
-        <v>0</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="12" t="n">
+      <c r="A41" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B41" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="B41" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C41" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D41" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E41" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="F41" s="12" t="n">
-        <v>0</v>
-      </c>
+      <c r="F41" s="12"/>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="12"/>
-      <c r="B42" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="C42" s="6"/>
-      <c r="D42" s="7"/>
-      <c r="E42" s="8"/>
-      <c r="F42" s="22"/>
+      <c r="A42" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B42" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="17"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="19" t="n">
+        <v>3</v>
+      </c>
+      <c r="F42" s="19"/>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="B43" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C43" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D43" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E43" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="F43" s="12" t="n">
-        <v>0</v>
-      </c>
+      <c r="A43" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="17"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F43" s="19"/>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B44" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="C44" s="10"/>
-      <c r="D44" s="11" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="E44" s="23" t="n">
-        <v>1</v>
-      </c>
-      <c r="F44" s="12" t="n">
-        <v>2</v>
-      </c>
+      <c r="A44" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F44" s="19"/>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="12" t="n">
-        <v>3</v>
-      </c>
-      <c r="B45" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="C45" s="10" t="s">
-        <v>59</v>
-      </c>
-      <c r="D45" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E45" s="23" t="n">
+      <c r="A45" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="17"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" s="19"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46" s="21" t="s">
+        <v>54</v>
+      </c>
+      <c r="D46" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E46" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F46" s="12" t="n">
         <v>1.5</v>
       </c>
-      <c r="F45" s="12" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="12"/>
-      <c r="B46" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="C46" s="6"/>
-      <c r="D46" s="7"/>
-      <c r="E46" s="8"/>
-      <c r="F46" s="22"/>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="12" t="n">
@@ -1613,10 +1637,10 @@
         <v>2</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C48" s="25" t="s">
-        <v>67</v>
+        <v>63</v>
+      </c>
+      <c r="C48" s="23" t="s">
+        <v>64</v>
       </c>
       <c r="D48" s="11" t="n">
         <v>1</v>
@@ -1629,49 +1653,49 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="26"/>
-      <c r="C49" s="26"/>
-      <c r="E49" s="27" t="n">
+      <c r="B49" s="24"/>
+      <c r="C49" s="24"/>
+      <c r="E49" s="25" t="n">
         <f aca="false">SUM(E38:E48)</f>
-        <v>7</v>
-      </c>
-      <c r="F49" s="27" t="n">
+        <v>11.5</v>
+      </c>
+      <c r="F49" s="25" t="n">
         <f aca="false">SUM(F38:F48)</f>
-        <v>5.5</v>
+        <v>5.75</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="26"/>
-      <c r="C50" s="26"/>
-      <c r="E50" s="27"/>
-      <c r="F50" s="27"/>
+      <c r="B50" s="24"/>
+      <c r="C50" s="24"/>
+      <c r="E50" s="25"/>
+      <c r="F50" s="25"/>
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B52" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C52" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D52" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="B51" s="1" t="s">
+      <c r="E52" s="26" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B52" s="28" t="s">
+      <c r="F52" s="26" t="s">
         <v>70</v>
-      </c>
-      <c r="C52" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D52" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E52" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="F52" s="28" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1689,10 +1713,10 @@
         <v>1</v>
       </c>
       <c r="B54" s="15" t="s">
-        <v>58</v>
+        <v>71</v>
       </c>
       <c r="C54" s="10" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D54" s="11" t="n">
         <v>0</v>
@@ -1709,10 +1733,10 @@
         <v>2</v>
       </c>
       <c r="B55" s="15" t="s">
-        <v>60</v>
+        <v>73</v>
       </c>
       <c r="C55" s="10" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D55" s="11" t="n">
         <v>0</v>
@@ -1729,10 +1753,10 @@
         <v>3</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>61</v>
+        <v>74</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D56" s="11" t="n">
         <v>0</v>
@@ -1747,7 +1771,7 @@
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="12"/>
       <c r="B57" s="5" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="7"/>
@@ -1759,15 +1783,15 @@
         <v>1</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="D58" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E58" s="23" t="n">
+      <c r="E58" s="27" t="n">
         <v>2</v>
       </c>
       <c r="F58" s="12" t="n">
@@ -1789,15 +1813,15 @@
         <v>1</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D60" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E60" s="23" t="n">
+      <c r="E60" s="27" t="n">
         <v>0</v>
       </c>
       <c r="F60" s="12" t="n">
@@ -1806,7 +1830,7 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="12"/>
-      <c r="B61" s="24" t="s">
+      <c r="B61" s="28" t="s">
         <v>52</v>
       </c>
       <c r="C61" s="6"/>
@@ -1839,10 +1863,10 @@
         <v>2</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>66</v>
-      </c>
-      <c r="C63" s="25" t="s">
-        <v>77</v>
+        <v>63</v>
+      </c>
+      <c r="C63" s="23" t="s">
+        <v>78</v>
       </c>
       <c r="D63" s="11" t="n">
         <v>1</v>
@@ -1855,49 +1879,49 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="26"/>
-      <c r="C64" s="26"/>
-      <c r="E64" s="27" t="n">
+      <c r="B64" s="24"/>
+      <c r="C64" s="24"/>
+      <c r="E64" s="25" t="n">
         <f aca="false">SUM(E53:E63)</f>
         <v>8</v>
       </c>
-      <c r="F64" s="27" t="n">
+      <c r="F64" s="25" t="n">
         <f aca="false">SUM(F53:F63)</f>
         <v>6.5</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="26"/>
-      <c r="C65" s="26"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
+      <c r="B65" s="24"/>
+      <c r="C65" s="24"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="25"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
         <v>56</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B67" s="28" t="s">
+      <c r="A67" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C67" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D67" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E67" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F67" s="26" t="s">
         <v>70</v>
-      </c>
-      <c r="C67" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D67" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E67" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="F67" s="28" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1995,10 +2019,10 @@
         <v>5</v>
       </c>
       <c r="B73" s="15" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="C73" s="10" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D73" s="11" t="n">
         <v>1</v>
@@ -2053,7 +2077,7 @@
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="12"/>
       <c r="B76" s="5" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C76" s="6"/>
       <c r="D76" s="7"/>
@@ -2065,15 +2089,15 @@
         <v>1</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C77" s="21" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D77" s="11" t="n">
         <v>0.7</v>
       </c>
-      <c r="E77" s="23" t="n">
+      <c r="E77" s="27" t="n">
         <v>2</v>
       </c>
       <c r="F77" s="12" t="n">
@@ -2095,15 +2119,15 @@
         <v>1</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D79" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E79" s="23" t="n">
+      <c r="E79" s="27" t="n">
         <v>1.5</v>
       </c>
       <c r="F79" s="12" t="n">
@@ -2112,7 +2136,7 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="12"/>
-      <c r="B80" s="24" t="s">
+      <c r="B80" s="28" t="s">
         <v>52</v>
       </c>
       <c r="C80" s="6"/>
@@ -2147,8 +2171,8 @@
       <c r="B82" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C82" s="25" t="s">
-        <v>83</v>
+      <c r="C82" s="23" t="s">
+        <v>84</v>
       </c>
       <c r="D82" s="11" t="n">
         <v>1</v>
@@ -2161,13 +2185,13 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="26"/>
-      <c r="C83" s="26"/>
-      <c r="E83" s="27" t="n">
+      <c r="B83" s="24"/>
+      <c r="C83" s="24"/>
+      <c r="E83" s="25" t="n">
         <f aca="false">SUM(E68:E82)</f>
         <v>8</v>
       </c>
-      <c r="F83" s="27" t="n">
+      <c r="F83" s="25" t="n">
         <f aca="false">SUM(F68:F82)</f>
         <v>6.6</v>
       </c>
@@ -2177,27 +2201,27 @@
         <v>42</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B86" s="28" t="s">
+      <c r="A86" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C86" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D86" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E86" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F86" s="26" t="s">
         <v>70</v>
-      </c>
-      <c r="C86" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D86" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E86" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="F86" s="28" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2215,7 +2239,7 @@
         <v>1</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C88" s="10" t="s">
         <v>22</v>
@@ -2235,7 +2259,7 @@
         <v>2</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>24</v>
@@ -2255,7 +2279,7 @@
         <v>3</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>27</v>
@@ -2275,7 +2299,7 @@
         <v>4</v>
       </c>
       <c r="B91" s="15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>29</v>
@@ -2295,7 +2319,7 @@
         <v>5</v>
       </c>
       <c r="B92" s="15" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>31</v>
@@ -2333,7 +2357,7 @@
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="12"/>
       <c r="B94" s="5" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C94" s="6"/>
       <c r="D94" s="7"/>
@@ -2345,15 +2369,15 @@
         <v>1</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C95" s="21" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="D95" s="11" t="n">
         <v>0.4</v>
       </c>
-      <c r="E95" s="23" t="n">
+      <c r="E95" s="27" t="n">
         <v>2</v>
       </c>
       <c r="F95" s="12" t="n">
@@ -2378,12 +2402,12 @@
         <v>53</v>
       </c>
       <c r="C97" s="21" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D97" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E97" s="23" t="n">
+      <c r="E97" s="27" t="n">
         <v>0.5</v>
       </c>
       <c r="F97" s="12" t="n">
@@ -2405,15 +2429,15 @@
         <v>1</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D99" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E99" s="23" t="n">
+      <c r="E99" s="27" t="n">
         <v>1</v>
       </c>
       <c r="F99" s="12" t="n">
@@ -2422,7 +2446,7 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="12"/>
-      <c r="B100" s="24" t="s">
+      <c r="B100" s="28" t="s">
         <v>52</v>
       </c>
       <c r="C100" s="6"/>
@@ -2457,8 +2481,8 @@
       <c r="B102" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C102" s="25" t="s">
-        <v>91</v>
+      <c r="C102" s="23" t="s">
+        <v>92</v>
       </c>
       <c r="D102" s="11" t="n">
         <v>1</v>
@@ -2471,43 +2495,43 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="26"/>
-      <c r="C103" s="26"/>
-      <c r="E103" s="27" t="n">
+      <c r="B103" s="24"/>
+      <c r="C103" s="24"/>
+      <c r="E103" s="25" t="n">
         <f aca="false">SUM(E87:E102)</f>
         <v>8.25</v>
       </c>
-      <c r="F103" s="27" t="n">
+      <c r="F103" s="25" t="n">
         <f aca="false">SUM(F87:F102)</f>
         <v>6.75</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B106" s="28" t="s">
+      <c r="A106" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C106" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D106" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E106" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F106" s="26" t="s">
         <v>70</v>
-      </c>
-      <c r="C106" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D106" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E106" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="F106" s="28" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2525,7 +2549,7 @@
         <v>1</v>
       </c>
       <c r="B108" s="15" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>10</v>
@@ -2545,7 +2569,7 @@
         <v>2</v>
       </c>
       <c r="B109" s="15" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="C109" s="10" t="s">
         <v>12</v>
@@ -2565,7 +2589,7 @@
         <v>3</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="C110" s="10" t="s">
         <v>14</v>
@@ -2585,7 +2609,7 @@
         <v>4</v>
       </c>
       <c r="B111" s="15" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="C111" s="10" t="s">
         <v>17</v>
@@ -2605,7 +2629,7 @@
         <v>5</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C112" s="10" t="s">
         <v>19</v>
@@ -2625,10 +2649,10 @@
         <v>6</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C113" s="10" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D113" s="11" t="n">
         <v>1</v>
@@ -2643,7 +2667,7 @@
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="12"/>
       <c r="B114" s="5" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C114" s="6"/>
       <c r="D114" s="7"/>
@@ -2655,15 +2679,15 @@
         <v>1</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="C115" s="21" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D115" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E115" s="23" t="n">
+      <c r="E115" s="27" t="n">
         <v>2</v>
       </c>
       <c r="F115" s="12" t="n">
@@ -2688,10 +2712,10 @@
         <v>53</v>
       </c>
       <c r="C117" s="21" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="D117" s="11"/>
-      <c r="E117" s="23" t="n">
+      <c r="E117" s="27" t="n">
         <v>0</v>
       </c>
       <c r="F117" s="12" t="n">
@@ -2713,15 +2737,15 @@
         <v>1</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C119" s="21" t="s">
-        <v>59</v>
+        <v>72</v>
       </c>
       <c r="D119" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E119" s="23" t="n">
+      <c r="E119" s="27" t="n">
         <v>1</v>
       </c>
       <c r="F119" s="12" t="n">
@@ -2730,7 +2754,7 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="12"/>
-      <c r="B120" s="24" t="s">
+      <c r="B120" s="28" t="s">
         <v>52</v>
       </c>
       <c r="C120" s="6"/>
@@ -2765,8 +2789,8 @@
       <c r="B122" s="10" t="s">
         <v>52</v>
       </c>
-      <c r="C122" s="25" t="s">
-        <v>103</v>
+      <c r="C122" s="23" t="s">
+        <v>104</v>
       </c>
       <c r="D122" s="11" t="n">
         <v>1</v>
@@ -2779,13 +2803,13 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B123" s="26"/>
-      <c r="C123" s="26"/>
-      <c r="E123" s="27" t="n">
+      <c r="B123" s="24"/>
+      <c r="C123" s="24"/>
+      <c r="E123" s="25" t="n">
         <f aca="false">SUM(E107:E122)</f>
         <v>7.75</v>
       </c>
-      <c r="F123" s="27" t="n">
+      <c r="F123" s="25" t="n">
         <f aca="false">SUM(F107:F122)</f>
         <v>6.75</v>
       </c>
@@ -2800,31 +2824,29 @@
     <hyperlink ref="B21" r:id="rId6" display="Void pointers"/>
     <hyperlink ref="B22" r:id="rId7" display="Pointers to pointers and dynamic multidimensional arrays"/>
     <hyperlink ref="B31" r:id="rId8" display="Pointers to pointers and dynamic multidimensional arrays"/>
-    <hyperlink ref="B39" r:id="rId9" display="An introduction to std::array"/>
-    <hyperlink ref="B40" r:id="rId10" display="An introduction to std::vector"/>
-    <hyperlink ref="B41" r:id="rId11" display="Chapter 6 comprehensive quiz"/>
-    <hyperlink ref="B54" r:id="rId12" display="An introduction to std::array"/>
-    <hyperlink ref="B55" r:id="rId13" display="An introduction to std::vector"/>
-    <hyperlink ref="B56" r:id="rId14" display="Chapter 6 comprehensive quiz"/>
-    <hyperlink ref="B69" r:id="rId15" display="Pointers and const"/>
-    <hyperlink ref="B70" r:id="rId16" display="Reference variables"/>
-    <hyperlink ref="B71" r:id="rId17" display="References and const"/>
-    <hyperlink ref="B72" r:id="rId18" display="Member selection with pointers and references"/>
-    <hyperlink ref="B73" r:id="rId19" display="For each loops"/>
-    <hyperlink ref="B74" r:id="rId20" display="Void pointers"/>
-    <hyperlink ref="B75" r:id="rId21" display="Pointers to pointers and dynamic multidimensional arrays"/>
-    <hyperlink ref="B88" r:id="rId22" display="Null pointers"/>
-    <hyperlink ref="B89" r:id="rId23" display="Pointers and arrays"/>
-    <hyperlink ref="B90" r:id="rId24" display="Pointer arithmetic and array indexing"/>
-    <hyperlink ref="B91" r:id="rId25" display="C-style string symbolic constants"/>
-    <hyperlink ref="B92" r:id="rId26" display="Dynamic memory allocation with new and delete"/>
-    <hyperlink ref="B93" r:id="rId27" display="Dynamically allocating arrays"/>
-    <hyperlink ref="B108" r:id="rId28" display="Arrays (Part II)and (Part I)"/>
-    <hyperlink ref="B109" r:id="rId29" display="Arrays and loops"/>
-    <hyperlink ref="B110" r:id="rId30" display="Sorting an array using selection sort"/>
-    <hyperlink ref="B111" r:id="rId31" display="Multidimensional arrays"/>
-    <hyperlink ref="B112" r:id="rId32" display="C-style strings"/>
-    <hyperlink ref="B113" r:id="rId33" display="Introduction to pointers"/>
+    <hyperlink ref="B40" r:id="rId9" display="Pointers to pointers and dynamic multidimensional arrays"/>
+    <hyperlink ref="B54" r:id="rId10" display="An introduction to std::array"/>
+    <hyperlink ref="B55" r:id="rId11" display="An introduction to std::vector"/>
+    <hyperlink ref="B56" r:id="rId12" display="Chapter 6 comprehensive quiz"/>
+    <hyperlink ref="B69" r:id="rId13" display="Pointers and const"/>
+    <hyperlink ref="B70" r:id="rId14" display="Reference variables"/>
+    <hyperlink ref="B71" r:id="rId15" display="References and const"/>
+    <hyperlink ref="B72" r:id="rId16" display="Member selection with pointers and references"/>
+    <hyperlink ref="B73" r:id="rId17" display="For each loops"/>
+    <hyperlink ref="B74" r:id="rId18" display="Void pointers"/>
+    <hyperlink ref="B75" r:id="rId19" display="Pointers to pointers and dynamic multidimensional arrays"/>
+    <hyperlink ref="B88" r:id="rId20" display="Null pointers"/>
+    <hyperlink ref="B89" r:id="rId21" display="Pointers and arrays"/>
+    <hyperlink ref="B90" r:id="rId22" display="Pointer arithmetic and array indexing"/>
+    <hyperlink ref="B91" r:id="rId23" display="C-style string symbolic constants"/>
+    <hyperlink ref="B92" r:id="rId24" display="Dynamic memory allocation with new and delete"/>
+    <hyperlink ref="B93" r:id="rId25" display="Dynamically allocating arrays"/>
+    <hyperlink ref="B108" r:id="rId26" display="Arrays (Part II)and (Part I)"/>
+    <hyperlink ref="B109" r:id="rId27" display="Arrays and loops"/>
+    <hyperlink ref="B110" r:id="rId28" display="Sorting an array using selection sort"/>
+    <hyperlink ref="B111" r:id="rId29" display="Multidimensional arrays"/>
+    <hyperlink ref="B112" r:id="rId30" display="C-style strings"/>
+    <hyperlink ref="B113" r:id="rId31" display="Introduction to pointers"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -2841,31 +2863,30 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H37"/>
+  <dimension ref="A1:H46"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A30" activeCellId="0" sqref="A30"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="45.4897959183674"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="34.1530612244898"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.8265306122449"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.3622448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="11.6071428571429"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="23.6224489795918"/>
-    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.7397959183673"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8010204081633"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9591836734694"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.6785714285714"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2885,13 +2906,13 @@
         <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7"/>
@@ -2911,7 +2932,8 @@
         <v>3</v>
       </c>
       <c r="F4" s="12" t="n">
-        <v>4</v>
+        <f aca="false">4+2</f>
+        <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2926,7 +2948,10 @@
       <c r="E5" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="F5" s="12"/>
+      <c r="F5" s="12" t="n">
+        <f aca="false">3</f>
+        <v>3</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="n">
@@ -3052,7 +3077,7 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
       <c r="B15" s="31" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="7"/>
@@ -3072,7 +3097,8 @@
         <v>2.5</v>
       </c>
       <c r="F16" s="12" t="n">
-        <v>0.5</v>
+        <f aca="false">0.5+0.5</f>
+        <v>1</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3088,7 +3114,8 @@
         <v>5</v>
       </c>
       <c r="F17" s="12" t="n">
-        <v>1</v>
+        <f aca="false">1+1.5</f>
+        <v>2.5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3096,7 +3123,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
@@ -3114,7 +3141,7 @@
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">SUM(F3:F18)</f>
-        <v>5.5</v>
+        <v>12.5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3122,30 +3149,30 @@
         <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="28" t="s">
+      <c r="A22" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D22" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F22" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="C22" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D22" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E22" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="F22" s="28" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="23" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="12" t="n">
         <v>1</v>
       </c>
@@ -3242,13 +3269,13 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="26"/>
-      <c r="C28" s="26"/>
-      <c r="E28" s="27" t="n">
+      <c r="B28" s="24"/>
+      <c r="C28" s="24"/>
+      <c r="E28" s="25" t="n">
         <f aca="false">SUM(E23:E27)</f>
         <v>8</v>
       </c>
-      <c r="F28" s="27" t="n">
+      <c r="F28" s="25" t="n">
         <f aca="false">SUM(F23:F27)</f>
         <v>5.5</v>
       </c>
@@ -3262,23 +3289,23 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="28" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="28" t="s">
+      <c r="A31" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D31" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F31" s="26" t="s">
         <v>70</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>71</v>
-      </c>
-      <c r="D31" s="28" t="s">
-        <v>72</v>
-      </c>
-      <c r="E31" s="28" t="s">
-        <v>73</v>
-      </c>
-      <c r="F31" s="28" t="s">
-        <v>74</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3288,26 +3315,38 @@
       <c r="B32" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="16"/>
-      <c r="D32" s="11"/>
+      <c r="C32" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="D32" s="11" t="n">
+        <v>1</v>
+      </c>
       <c r="E32" s="12" t="n">
         <v>1.5</v>
       </c>
-      <c r="F32" s="12"/>
+      <c r="F32" s="12" t="n">
+        <v>2</v>
+      </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="12" t="n">
         <v>2</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="C33" s="17"/>
-      <c r="D33" s="18"/>
+        <v>59</v>
+      </c>
+      <c r="C33" s="17" t="s">
+        <v>60</v>
+      </c>
+      <c r="D33" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="E33" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F33" s="19"/>
+      <c r="F33" s="19" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="12" t="n">
@@ -3330,12 +3369,18 @@
       <c r="B35" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C35" s="17"/>
-      <c r="D35" s="18"/>
+      <c r="C35" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="D35" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="E35" s="33" t="n">
         <v>0.5</v>
       </c>
-      <c r="F35" s="19"/>
+      <c r="F35" s="19" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="12" t="n">
@@ -3344,22 +3389,138 @@
       <c r="B36" s="20" t="s">
         <v>52</v>
       </c>
-      <c r="C36" s="17"/>
-      <c r="D36" s="18"/>
+      <c r="C36" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D36" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="E36" s="19" t="n">
         <v>2</v>
       </c>
-      <c r="F36" s="32"/>
+      <c r="F36" s="32" t="n">
+        <v>1.5</v>
+      </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="26"/>
-      <c r="C37" s="26"/>
-      <c r="E37" s="27" t="n">
+      <c r="B37" s="24"/>
+      <c r="C37" s="24"/>
+      <c r="E37" s="25" t="n">
         <f aca="false">SUM(E32:E36)</f>
         <v>8</v>
       </c>
-      <c r="F37" s="27" t="n">
+      <c r="F37" s="25" t="n">
         <f aca="false">SUM(F32:F36)</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="26" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="26" t="s">
+        <v>66</v>
+      </c>
+      <c r="C40" s="26" t="s">
+        <v>67</v>
+      </c>
+      <c r="D40" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="E40" s="26" t="s">
+        <v>69</v>
+      </c>
+      <c r="F40" s="26" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B41" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="16"/>
+      <c r="D41" s="11"/>
+      <c r="E41" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="F41" s="12"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B42" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C42" s="17"/>
+      <c r="D42" s="18"/>
+      <c r="E42" s="19" t="n">
+        <v>3</v>
+      </c>
+      <c r="F42" s="19"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B43" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="C43" s="17"/>
+      <c r="D43" s="18"/>
+      <c r="E43" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F43" s="32"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="B44" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44" s="17"/>
+      <c r="D44" s="18"/>
+      <c r="E44" s="33" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F44" s="19"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="B45" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45" s="17"/>
+      <c r="D45" s="18"/>
+      <c r="E45" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F45" s="32"/>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B46" s="24"/>
+      <c r="C46" s="24"/>
+      <c r="E46" s="25" t="n">
+        <f aca="false">SUM(E41:E45)</f>
+        <v>8</v>
+      </c>
+      <c r="F46" s="25" t="n">
+        <f aca="false">SUM(F41:F45)</f>
         <v>0</v>
       </c>
     </row>
@@ -3387,34 +3548,34 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="56.4285714285714"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.5357142857143"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="34" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="57.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="46.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="35" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="35" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
31 Oct 2019 SLL (single Linked List)
</commit_message>
<xml_diff>
--- a/Daily_plan/2019/10_Oct/29-Oct_01-Nov.xlsx
+++ b/Daily_plan/2019/10_Oct/29-Oct_01-Nov.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="326" uniqueCount="115">
   <si>
     <t xml:space="preserve">Week_03</t>
   </si>
@@ -176,6 +176,9 @@
     <t xml:space="preserve">Data Structure: Queue in C++</t>
   </si>
   <si>
+    <t xml:space="preserve">NYS</t>
+  </si>
+  <si>
     <t xml:space="preserve">Python: OOPs</t>
   </si>
   <si>
@@ -215,13 +218,34 @@
     <t xml:space="preserve">31-10-2019</t>
   </si>
   <si>
+    <t xml:space="preserve">completed coding the SLL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fri</t>
+  </si>
+  <si>
+    <t xml:space="preserve">01-11-2019</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chapter 6 comprehensive quiz</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Data Structure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Queue using linked list using C</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tutorial</t>
+  </si>
+  <si>
     <t xml:space="preserve">Miscellaneous Activity (Knowledge updation based on CV)</t>
   </si>
   <si>
-    <t xml:space="preserve">Went through C++ basic, Attended online test</t>
-  </si>
-  <si>
-    <t xml:space="preserve">20-06-2019</t>
+    <t xml:space="preserve">Revised the project and technical part and went through the C++ topics</t>
+  </si>
+  <si>
+    <t xml:space="preserve">19-06-2019</t>
   </si>
   <si>
     <t xml:space="preserve">Daily Task                        </t>
@@ -237,33 +261,6 @@
   </si>
   <si>
     <t xml:space="preserve">Actual Hrs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An introduction to std::array</t>
-  </si>
-  <si>
-    <t xml:space="preserve">NYS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">An introduction to std::vector</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Chapter 6 comprehensive quiz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Data Structure</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Queue using linked list using C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tutorial</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Revised the project and technical part and went through the C++ topics</t>
-  </si>
-  <si>
-    <t xml:space="preserve">19-06-2019</t>
   </si>
   <si>
     <t xml:space="preserve">For each loops</t>
@@ -515,14 +512,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC00"/>
-        <bgColor rgb="FFFFFF00"/>
+        <fgColor rgb="FF669900"/>
+        <bgColor rgb="FF339966"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF669900"/>
-        <bgColor rgb="FF339966"/>
+        <fgColor rgb="FFFFCC00"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -661,6 +658,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -672,16 +677,8 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -692,7 +689,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="8" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="7" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -797,14 +794,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.6632653061225"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.8775510204082"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.71938775510204"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.23469387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.44897959183673"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -903,7 +900,10 @@
       <c r="E6" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="F6" s="12" t="n">
+        <f aca="false">4.5</f>
+        <v>4.5</v>
+      </c>
       <c r="H6" s="13" t="s">
         <v>15</v>
       </c>
@@ -1079,8 +1079,8 @@
         <v>0.5</v>
       </c>
       <c r="F16" s="12" t="n">
-        <f aca="false">0.5+0.5</f>
-        <v>1</v>
+        <f aca="false">0.5+0.5+0.5</f>
+        <v>1.5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1100,8 +1100,8 @@
         <v>0.5</v>
       </c>
       <c r="F17" s="12" t="n">
-        <f aca="false">1+1.5</f>
-        <v>2.5</v>
+        <f aca="false">1+1.5+1</f>
+        <v>3.5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1142,6 +1142,10 @@
       </c>
       <c r="F19" s="12" t="n">
         <v>0.1</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <f aca="false">F28+F37+F46</f>
+        <v>4.5</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1219,7 +1223,9 @@
       <c r="B24" s="15" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="17" t="s">
+        <v>50</v>
+      </c>
       <c r="D24" s="18" t="n">
         <v>0</v>
       </c>
@@ -1235,9 +1241,11 @@
         <v>3</v>
       </c>
       <c r="B25" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="17"/>
       <c r="D25" s="18" t="n">
         <v>0</v>
       </c>
@@ -1253,10 +1261,10 @@
         <v>4</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D26" s="18" t="n">
         <v>1</v>
@@ -1273,10 +1281,10 @@
         <v>5</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D27" s="18" t="n">
         <v>1</v>
@@ -1293,10 +1301,10 @@
         <v>1</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C28" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D28" s="11" t="n">
         <v>1</v>
@@ -1311,7 +1319,7 @@
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4"/>
       <c r="B29" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C29" s="6"/>
       <c r="D29" s="7"/>
@@ -1320,10 +1328,10 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>44</v>
@@ -1366,7 +1374,7 @@
         <v>47</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D32" s="11" t="n">
         <v>1</v>
@@ -1383,10 +1391,10 @@
         <v>2</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D33" s="18" t="n">
         <v>1</v>
@@ -1403,9 +1411,11 @@
         <v>3</v>
       </c>
       <c r="B34" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="17"/>
       <c r="D34" s="18"/>
       <c r="E34" s="19" t="n">
         <v>1</v>
@@ -1417,10 +1427,10 @@
         <v>4</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D35" s="18" t="n">
         <v>1</v>
@@ -1437,10 +1447,10 @@
         <v>5</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D36" s="18" t="n">
         <v>1</v>
@@ -1457,10 +1467,10 @@
         <v>1</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D37" s="11" t="n">
         <v>1</v>
@@ -1484,10 +1494,10 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B39" s="15" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>44</v>
@@ -1529,12 +1539,18 @@
       <c r="B41" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="11"/>
+      <c r="C41" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="11" t="n">
+        <v>0.9</v>
+      </c>
       <c r="E41" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="F41" s="12"/>
+      <c r="F41" s="12" t="n">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="4" t="n">
@@ -1543,64 +1559,88 @@
       <c r="B42" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="18"/>
+      <c r="C42" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="18" t="n">
+        <v>0</v>
+      </c>
       <c r="E42" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F42" s="19"/>
+      <c r="F42" s="19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="4" t="n">
         <v>3</v>
       </c>
       <c r="B43" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="17"/>
-      <c r="D43" s="18"/>
+      <c r="D43" s="18" t="n">
+        <v>0</v>
+      </c>
       <c r="E43" s="19" t="n">
         <v>0.5</v>
       </c>
-      <c r="F43" s="19"/>
+      <c r="F43" s="19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="4" t="n">
         <v>4</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" s="17"/>
-      <c r="D44" s="18"/>
+        <v>52</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="E44" s="19" t="n">
         <v>0.5</v>
       </c>
-      <c r="F44" s="19"/>
+      <c r="F44" s="19" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="4" t="n">
         <v>5</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="18"/>
+        <v>53</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="E45" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="F45" s="19"/>
+      <c r="F45" s="19" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B46" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C46" s="21" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D46" s="11" t="n">
         <v>1</v>
@@ -1617,135 +1657,149 @@
         <v>1</v>
       </c>
       <c r="B47" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="C47" s="10" t="s">
+        <v>52</v>
+      </c>
+      <c r="D47" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" s="12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F47" s="12" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C48" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D48" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E48" s="12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F48" s="12" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="4" t="n">
+        <v>19</v>
+      </c>
+      <c r="B49" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="C49" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D49" s="11" t="n">
+        <v>1</v>
+      </c>
+      <c r="E49" s="12" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F49" s="12" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B50" s="9" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="16"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" s="12"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="B51" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="17"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="F51" s="19"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="B52" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="C47" s="10" t="s">
-        <v>51</v>
-      </c>
-      <c r="D47" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E47" s="12" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F47" s="12" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B48" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C48" s="23" t="s">
-        <v>64</v>
-      </c>
-      <c r="D48" s="11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E48" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="F48" s="12" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="24"/>
-      <c r="C49" s="24"/>
-      <c r="E49" s="25" t="n">
-        <f aca="false">SUM(E38:E48)</f>
-        <v>11.5</v>
-      </c>
-      <c r="F49" s="25" t="n">
-        <f aca="false">SUM(F38:F48)</f>
-        <v>5.75</v>
-      </c>
-    </row>
-    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="24"/>
-      <c r="C50" s="24"/>
-      <c r="E50" s="25"/>
-      <c r="F50" s="25"/>
-    </row>
-    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A51" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B51" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B52" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C52" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D52" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E52" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="F52" s="26" t="s">
-        <v>70</v>
-      </c>
+      <c r="C52" s="17"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F52" s="19"/>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="12"/>
-      <c r="B53" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="6"/>
-      <c r="D53" s="7"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="22"/>
+      <c r="A53" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="17"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F53" s="19"/>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="12" t="n">
-        <v>1</v>
-      </c>
-      <c r="B54" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C54" s="10" t="s">
-        <v>72</v>
-      </c>
-      <c r="D54" s="11" t="n">
-        <v>0</v>
-      </c>
-      <c r="E54" s="12" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F54" s="12" t="n">
-        <v>0</v>
-      </c>
+      <c r="A54" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="17"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F54" s="19"/>
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="12" t="n">
-        <v>2</v>
-      </c>
-      <c r="B55" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C55" s="10" t="s">
-        <v>72</v>
+      <c r="A55" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="B55" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>55</v>
       </c>
       <c r="D55" s="11" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E55" s="12" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F55" s="12" t="n">
-        <v>0</v>
+        <v>1.5</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1753,10 +1807,10 @@
         <v>3</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>74</v>
+        <v>67</v>
       </c>
       <c r="C56" s="10" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D56" s="11" t="n">
         <v>0</v>
@@ -1771,7 +1825,7 @@
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="12"/>
       <c r="B57" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C57" s="6"/>
       <c r="D57" s="7"/>
@@ -1783,15 +1837,15 @@
         <v>1</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C58" s="10" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="D58" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E58" s="27" t="n">
+      <c r="E58" s="23" t="n">
         <v>2</v>
       </c>
       <c r="F58" s="12" t="n">
@@ -1801,7 +1855,7 @@
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="12"/>
       <c r="B59" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C59" s="6"/>
       <c r="D59" s="7"/>
@@ -1813,15 +1867,15 @@
         <v>1</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C60" s="10" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D60" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E60" s="27" t="n">
+      <c r="E60" s="23" t="n">
         <v>0</v>
       </c>
       <c r="F60" s="12" t="n">
@@ -1830,8 +1884,8 @@
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="12"/>
-      <c r="B61" s="28" t="s">
-        <v>52</v>
+      <c r="B61" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="C61" s="6"/>
       <c r="D61" s="7"/>
@@ -1843,10 +1897,10 @@
         <v>1</v>
       </c>
       <c r="B62" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C62" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D62" s="11" t="n">
         <v>1</v>
@@ -1863,10 +1917,10 @@
         <v>2</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="C63" s="23" t="s">
-        <v>78</v>
+        <v>71</v>
+      </c>
+      <c r="C63" s="25" t="s">
+        <v>72</v>
       </c>
       <c r="D63" s="11" t="n">
         <v>1</v>
@@ -1879,49 +1933,49 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B64" s="24"/>
-      <c r="C64" s="24"/>
-      <c r="E64" s="25" t="n">
+      <c r="B64" s="26"/>
+      <c r="C64" s="26"/>
+      <c r="E64" s="27" t="n">
         <f aca="false">SUM(E53:E63)</f>
+        <v>9.5</v>
+      </c>
+      <c r="F64" s="27" t="n">
+        <f aca="false">SUM(F53:F63)</f>
         <v>8</v>
       </c>
-      <c r="F64" s="25" t="n">
-        <f aca="false">SUM(F53:F63)</f>
-        <v>6.5</v>
-      </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B65" s="24"/>
-      <c r="C65" s="24"/>
-      <c r="E65" s="25"/>
-      <c r="F65" s="25"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="26"/>
+      <c r="E65" s="27"/>
+      <c r="F65" s="27"/>
     </row>
     <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A66" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B66" s="1" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A67" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B67" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C67" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D67" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E67" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="F67" s="26" t="s">
-        <v>70</v>
+      <c r="A67" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B67" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C67" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D67" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E67" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="F67" s="28" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2019,10 +2073,10 @@
         <v>5</v>
       </c>
       <c r="B73" s="15" t="s">
+        <v>79</v>
+      </c>
+      <c r="C73" s="10" t="s">
         <v>80</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>81</v>
       </c>
       <c r="D73" s="11" t="n">
         <v>1</v>
@@ -2077,7 +2131,7 @@
     <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A76" s="12"/>
       <c r="B76" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C76" s="6"/>
       <c r="D76" s="7"/>
@@ -2089,15 +2143,15 @@
         <v>1</v>
       </c>
       <c r="B77" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C77" s="21" t="s">
         <v>82</v>
-      </c>
-      <c r="C77" s="21" t="s">
-        <v>83</v>
       </c>
       <c r="D77" s="11" t="n">
         <v>0.7</v>
       </c>
-      <c r="E77" s="27" t="n">
+      <c r="E77" s="23" t="n">
         <v>2</v>
       </c>
       <c r="F77" s="12" t="n">
@@ -2107,7 +2161,7 @@
     <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A78" s="12"/>
       <c r="B78" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C78" s="6"/>
       <c r="D78" s="7"/>
@@ -2119,15 +2173,15 @@
         <v>1</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C79" s="21" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D79" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E79" s="27" t="n">
+      <c r="E79" s="23" t="n">
         <v>1.5</v>
       </c>
       <c r="F79" s="12" t="n">
@@ -2136,8 +2190,8 @@
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A80" s="12"/>
-      <c r="B80" s="28" t="s">
-        <v>52</v>
+      <c r="B80" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="C80" s="6"/>
       <c r="D80" s="7"/>
@@ -2149,10 +2203,10 @@
         <v>1</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C81" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D81" s="11" t="n">
         <v>1</v>
@@ -2169,10 +2223,10 @@
         <v>2</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C82" s="23" t="s">
-        <v>84</v>
+        <v>53</v>
+      </c>
+      <c r="C82" s="25" t="s">
+        <v>83</v>
       </c>
       <c r="D82" s="11" t="n">
         <v>1</v>
@@ -2185,13 +2239,13 @@
       </c>
     </row>
     <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="24"/>
-      <c r="C83" s="24"/>
-      <c r="E83" s="25" t="n">
+      <c r="B83" s="26"/>
+      <c r="C83" s="26"/>
+      <c r="E83" s="27" t="n">
         <f aca="false">SUM(E68:E82)</f>
         <v>8</v>
       </c>
-      <c r="F83" s="25" t="n">
+      <c r="F83" s="27" t="n">
         <f aca="false">SUM(F68:F82)</f>
         <v>6.6</v>
       </c>
@@ -2201,27 +2255,27 @@
         <v>42</v>
       </c>
       <c r="B85" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A86" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B86" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C86" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D86" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E86" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="F86" s="26" t="s">
-        <v>70</v>
+      <c r="A86" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B86" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C86" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D86" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E86" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="F86" s="28" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2239,7 +2293,7 @@
         <v>1</v>
       </c>
       <c r="B88" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C88" s="10" t="s">
         <v>22</v>
@@ -2259,7 +2313,7 @@
         <v>2</v>
       </c>
       <c r="B89" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>24</v>
@@ -2279,7 +2333,7 @@
         <v>3</v>
       </c>
       <c r="B90" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>27</v>
@@ -2299,7 +2353,7 @@
         <v>4</v>
       </c>
       <c r="B91" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>29</v>
@@ -2319,7 +2373,7 @@
         <v>5</v>
       </c>
       <c r="B92" s="15" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>31</v>
@@ -2357,7 +2411,7 @@
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A94" s="12"/>
       <c r="B94" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C94" s="6"/>
       <c r="D94" s="7"/>
@@ -2369,15 +2423,15 @@
         <v>1</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C95" s="21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="D95" s="11" t="n">
         <v>0.4</v>
       </c>
-      <c r="E95" s="27" t="n">
+      <c r="E95" s="23" t="n">
         <v>2</v>
       </c>
       <c r="F95" s="12" t="n">
@@ -2399,15 +2453,15 @@
         <v>1</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C97" s="21" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D97" s="11" t="n">
         <v>1</v>
       </c>
-      <c r="E97" s="27" t="n">
+      <c r="E97" s="23" t="n">
         <v>0.5</v>
       </c>
       <c r="F97" s="12" t="n">
@@ -2417,7 +2471,7 @@
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A98" s="12"/>
       <c r="B98" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C98" s="6"/>
       <c r="D98" s="7"/>
@@ -2429,15 +2483,15 @@
         <v>1</v>
       </c>
       <c r="B99" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C99" s="21" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D99" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E99" s="27" t="n">
+      <c r="E99" s="23" t="n">
         <v>1</v>
       </c>
       <c r="F99" s="12" t="n">
@@ -2446,8 +2500,8 @@
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A100" s="12"/>
-      <c r="B100" s="28" t="s">
-        <v>52</v>
+      <c r="B100" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="C100" s="6"/>
       <c r="D100" s="7"/>
@@ -2459,10 +2513,10 @@
         <v>1</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C101" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D101" s="11" t="n">
         <v>1</v>
@@ -2479,10 +2533,10 @@
         <v>2</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C102" s="23" t="s">
-        <v>92</v>
+        <v>53</v>
+      </c>
+      <c r="C102" s="25" t="s">
+        <v>91</v>
       </c>
       <c r="D102" s="11" t="n">
         <v>1</v>
@@ -2495,43 +2549,43 @@
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="24"/>
-      <c r="C103" s="24"/>
-      <c r="E103" s="25" t="n">
+      <c r="B103" s="26"/>
+      <c r="C103" s="26"/>
+      <c r="E103" s="27" t="n">
         <f aca="false">SUM(E87:E102)</f>
         <v>8.25</v>
       </c>
-      <c r="F103" s="25" t="n">
+      <c r="F103" s="27" t="n">
         <f aca="false">SUM(F87:F102)</f>
         <v>6.75</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A105" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B105" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="B105" s="1" t="s">
-        <v>94</v>
-      </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A106" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B106" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C106" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D106" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E106" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="F106" s="26" t="s">
-        <v>70</v>
+      <c r="A106" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B106" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C106" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D106" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E106" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="F106" s="28" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2549,7 +2603,7 @@
         <v>1</v>
       </c>
       <c r="B108" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>10</v>
@@ -2569,7 +2623,7 @@
         <v>2</v>
       </c>
       <c r="B109" s="15" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C109" s="10" t="s">
         <v>12</v>
@@ -2589,7 +2643,7 @@
         <v>3</v>
       </c>
       <c r="B110" s="15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C110" s="10" t="s">
         <v>14</v>
@@ -2609,7 +2663,7 @@
         <v>4</v>
       </c>
       <c r="B111" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C111" s="10" t="s">
         <v>17</v>
@@ -2629,7 +2683,7 @@
         <v>5</v>
       </c>
       <c r="B112" s="15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C112" s="10" t="s">
         <v>19</v>
@@ -2649,10 +2703,10 @@
         <v>6</v>
       </c>
       <c r="B113" s="15" t="s">
+        <v>99</v>
+      </c>
+      <c r="C113" s="10" t="s">
         <v>100</v>
-      </c>
-      <c r="C113" s="10" t="s">
-        <v>101</v>
       </c>
       <c r="D113" s="11" t="n">
         <v>1</v>
@@ -2667,7 +2721,7 @@
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A114" s="12"/>
       <c r="B114" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C114" s="6"/>
       <c r="D114" s="7"/>
@@ -2679,15 +2733,15 @@
         <v>1</v>
       </c>
       <c r="B115" s="10" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C115" s="21" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D115" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E115" s="27" t="n">
+      <c r="E115" s="23" t="n">
         <v>2</v>
       </c>
       <c r="F115" s="12" t="n">
@@ -2709,13 +2763,13 @@
         <v>1</v>
       </c>
       <c r="B117" s="10" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="C117" s="21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="D117" s="11"/>
-      <c r="E117" s="27" t="n">
+      <c r="E117" s="23" t="n">
         <v>0</v>
       </c>
       <c r="F117" s="12" t="n">
@@ -2725,7 +2779,7 @@
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A118" s="12"/>
       <c r="B118" s="5" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C118" s="6"/>
       <c r="D118" s="7"/>
@@ -2737,15 +2791,15 @@
         <v>1</v>
       </c>
       <c r="B119" s="10" t="s">
-        <v>77</v>
+        <v>70</v>
       </c>
       <c r="C119" s="21" t="s">
-        <v>72</v>
+        <v>50</v>
       </c>
       <c r="D119" s="11" t="n">
         <v>0</v>
       </c>
-      <c r="E119" s="27" t="n">
+      <c r="E119" s="23" t="n">
         <v>1</v>
       </c>
       <c r="F119" s="12" t="n">
@@ -2754,8 +2808,8 @@
     </row>
     <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A120" s="12"/>
-      <c r="B120" s="28" t="s">
-        <v>52</v>
+      <c r="B120" s="24" t="s">
+        <v>53</v>
       </c>
       <c r="C120" s="6"/>
       <c r="D120" s="7"/>
@@ -2767,10 +2821,10 @@
         <v>1</v>
       </c>
       <c r="B121" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C121" s="10" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D121" s="11" t="n">
         <v>1</v>
@@ -2787,10 +2841,10 @@
         <v>2</v>
       </c>
       <c r="B122" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="C122" s="23" t="s">
-        <v>104</v>
+        <v>53</v>
+      </c>
+      <c r="C122" s="25" t="s">
+        <v>103</v>
       </c>
       <c r="D122" s="11" t="n">
         <v>1</v>
@@ -2803,13 +2857,13 @@
       </c>
     </row>
     <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B123" s="24"/>
-      <c r="C123" s="24"/>
-      <c r="E123" s="25" t="n">
+      <c r="B123" s="26"/>
+      <c r="C123" s="26"/>
+      <c r="E123" s="27" t="n">
         <f aca="false">SUM(E107:E122)</f>
         <v>7.75</v>
       </c>
-      <c r="F123" s="25" t="n">
+      <c r="F123" s="27" t="n">
         <f aca="false">SUM(F107:F122)</f>
         <v>6.75</v>
       </c>
@@ -2825,28 +2879,27 @@
     <hyperlink ref="B22" r:id="rId7" display="Pointers to pointers and dynamic multidimensional arrays"/>
     <hyperlink ref="B31" r:id="rId8" display="Pointers to pointers and dynamic multidimensional arrays"/>
     <hyperlink ref="B40" r:id="rId9" display="Pointers to pointers and dynamic multidimensional arrays"/>
-    <hyperlink ref="B54" r:id="rId10" display="An introduction to std::array"/>
-    <hyperlink ref="B55" r:id="rId11" display="An introduction to std::vector"/>
-    <hyperlink ref="B56" r:id="rId12" display="Chapter 6 comprehensive quiz"/>
-    <hyperlink ref="B69" r:id="rId13" display="Pointers and const"/>
-    <hyperlink ref="B70" r:id="rId14" display="Reference variables"/>
-    <hyperlink ref="B71" r:id="rId15" display="References and const"/>
-    <hyperlink ref="B72" r:id="rId16" display="Member selection with pointers and references"/>
-    <hyperlink ref="B73" r:id="rId17" display="For each loops"/>
-    <hyperlink ref="B74" r:id="rId18" display="Void pointers"/>
-    <hyperlink ref="B75" r:id="rId19" display="Pointers to pointers and dynamic multidimensional arrays"/>
-    <hyperlink ref="B88" r:id="rId20" display="Null pointers"/>
-    <hyperlink ref="B89" r:id="rId21" display="Pointers and arrays"/>
-    <hyperlink ref="B90" r:id="rId22" display="Pointer arithmetic and array indexing"/>
-    <hyperlink ref="B91" r:id="rId23" display="C-style string symbolic constants"/>
-    <hyperlink ref="B92" r:id="rId24" display="Dynamic memory allocation with new and delete"/>
-    <hyperlink ref="B93" r:id="rId25" display="Dynamically allocating arrays"/>
-    <hyperlink ref="B108" r:id="rId26" display="Arrays (Part II)and (Part I)"/>
-    <hyperlink ref="B109" r:id="rId27" display="Arrays and loops"/>
-    <hyperlink ref="B110" r:id="rId28" display="Sorting an array using selection sort"/>
-    <hyperlink ref="B111" r:id="rId29" display="Multidimensional arrays"/>
-    <hyperlink ref="B112" r:id="rId30" display="C-style strings"/>
-    <hyperlink ref="B113" r:id="rId31" display="Introduction to pointers"/>
+    <hyperlink ref="B49" r:id="rId10" display="Pointers to pointers and dynamic multidimensional arrays"/>
+    <hyperlink ref="B56" r:id="rId11" display="Chapter 6 comprehensive quiz"/>
+    <hyperlink ref="B69" r:id="rId12" display="Pointers and const"/>
+    <hyperlink ref="B70" r:id="rId13" display="Reference variables"/>
+    <hyperlink ref="B71" r:id="rId14" display="References and const"/>
+    <hyperlink ref="B72" r:id="rId15" display="Member selection with pointers and references"/>
+    <hyperlink ref="B73" r:id="rId16" display="For each loops"/>
+    <hyperlink ref="B74" r:id="rId17" display="Void pointers"/>
+    <hyperlink ref="B75" r:id="rId18" display="Pointers to pointers and dynamic multidimensional arrays"/>
+    <hyperlink ref="B88" r:id="rId19" display="Null pointers"/>
+    <hyperlink ref="B89" r:id="rId20" display="Pointers and arrays"/>
+    <hyperlink ref="B90" r:id="rId21" display="Pointer arithmetic and array indexing"/>
+    <hyperlink ref="B91" r:id="rId22" display="C-style string symbolic constants"/>
+    <hyperlink ref="B92" r:id="rId23" display="Dynamic memory allocation with new and delete"/>
+    <hyperlink ref="B93" r:id="rId24" display="Dynamically allocating arrays"/>
+    <hyperlink ref="B108" r:id="rId25" display="Arrays (Part II)and (Part I)"/>
+    <hyperlink ref="B109" r:id="rId26" display="Arrays and loops"/>
+    <hyperlink ref="B110" r:id="rId27" display="Sorting an array using selection sort"/>
+    <hyperlink ref="B111" r:id="rId28" display="Multidimensional arrays"/>
+    <hyperlink ref="B112" r:id="rId29" display="C-style strings"/>
+    <hyperlink ref="B113" r:id="rId30" display="Introduction to pointers"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
@@ -2863,30 +2916,29 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H46"/>
+  <dimension ref="A1:H55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A39" activeCellId="0" sqref="A39"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A49" activeCellId="0" sqref="A49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="43.7397959183673"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="32.8010204081633"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.9591836734694"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.6785714285714"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="42.6581632653061"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="31.9948979591837"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="12.1479591836735"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.6887755102041"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="0" width="22.1377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="9" style="0" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2906,13 +2958,13 @@
         <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4"/>
       <c r="B3" s="5" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="7"/>
@@ -2965,7 +3017,10 @@
       <c r="E6" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="F6" s="12"/>
+      <c r="F6" s="12" t="n">
+        <f aca="false">4.5</f>
+        <v>4.5</v>
+      </c>
       <c r="H6" s="13" t="s">
         <v>15</v>
       </c>
@@ -3077,7 +3132,7 @@
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="4"/>
       <c r="B15" s="31" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C15" s="6"/>
       <c r="D15" s="7"/>
@@ -3089,7 +3144,7 @@
         <v>1</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
@@ -3097,8 +3152,8 @@
         <v>2.5</v>
       </c>
       <c r="F16" s="12" t="n">
-        <f aca="false">0.5+0.5</f>
-        <v>1</v>
+        <f aca="false">0.5+0.5+0.5</f>
+        <v>1.5</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3106,7 +3161,7 @@
         <v>2</v>
       </c>
       <c r="B17" s="29" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
@@ -3114,8 +3169,8 @@
         <v>5</v>
       </c>
       <c r="F17" s="12" t="n">
-        <f aca="false">1+1.5</f>
-        <v>2.5</v>
+        <f aca="false">1+1.5+1</f>
+        <v>3.5</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3123,7 +3178,7 @@
         <v>3</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
@@ -3141,7 +3196,11 @@
       </c>
       <c r="F19" s="0" t="n">
         <f aca="false">SUM(F3:F18)</f>
-        <v>12.5</v>
+        <v>18.5</v>
+      </c>
+      <c r="H19" s="0" t="n">
+        <f aca="false">F28+F37+F46</f>
+        <v>18.5</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3149,27 +3208,27 @@
         <v>42</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B22" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C22" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D22" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E22" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="F22" s="26" t="s">
-        <v>70</v>
+      <c r="A22" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B22" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C22" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D22" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E22" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="F22" s="28" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3199,7 +3258,9 @@
       <c r="B24" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="C24" s="17"/>
+      <c r="C24" s="17" t="s">
+        <v>50</v>
+      </c>
       <c r="D24" s="18" t="n">
         <v>0</v>
       </c>
@@ -3215,9 +3276,11 @@
         <v>3</v>
       </c>
       <c r="B25" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C25" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C25" s="17"/>
       <c r="D25" s="18" t="n">
         <v>0</v>
       </c>
@@ -3233,10 +3296,10 @@
         <v>4</v>
       </c>
       <c r="B26" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C26" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D26" s="18" t="n">
         <v>1</v>
@@ -3253,10 +3316,10 @@
         <v>5</v>
       </c>
       <c r="B27" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D27" s="18" t="n">
         <v>1</v>
@@ -3269,43 +3332,43 @@
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="24"/>
-      <c r="C28" s="24"/>
-      <c r="E28" s="25" t="n">
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="E28" s="27" t="n">
         <f aca="false">SUM(E23:E27)</f>
         <v>8</v>
       </c>
-      <c r="F28" s="25" t="n">
+      <c r="F28" s="27" t="n">
         <f aca="false">SUM(F23:F27)</f>
         <v>5.5</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B31" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C31" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D31" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E31" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="F31" s="26" t="s">
-        <v>70</v>
+      <c r="A31" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B31" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C31" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D31" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E31" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3316,7 +3379,7 @@
         <v>47</v>
       </c>
       <c r="C32" s="16" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D32" s="11" t="n">
         <v>1</v>
@@ -3333,10 +3396,10 @@
         <v>2</v>
       </c>
       <c r="B33" s="20" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="C33" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D33" s="18" t="n">
         <v>1</v>
@@ -3353,9 +3416,11 @@
         <v>3</v>
       </c>
       <c r="B34" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C34" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="17"/>
       <c r="D34" s="18"/>
       <c r="E34" s="19" t="n">
         <v>1</v>
@@ -3367,10 +3432,10 @@
         <v>4</v>
       </c>
       <c r="B35" s="20" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C35" s="17" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="D35" s="18" t="n">
         <v>1</v>
@@ -3387,10 +3452,10 @@
         <v>5</v>
       </c>
       <c r="B36" s="20" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D36" s="18" t="n">
         <v>1</v>
@@ -3403,43 +3468,43 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="24"/>
-      <c r="C37" s="24"/>
-      <c r="E37" s="25" t="n">
+      <c r="B37" s="26"/>
+      <c r="C37" s="26"/>
+      <c r="E37" s="27" t="n">
         <f aca="false">SUM(E32:E36)</f>
         <v>8</v>
       </c>
-      <c r="F37" s="25" t="n">
+      <c r="F37" s="27" t="n">
         <f aca="false">SUM(F32:F36)</f>
         <v>7</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="26" t="s">
-        <v>2</v>
-      </c>
-      <c r="B40" s="26" t="s">
-        <v>66</v>
-      </c>
-      <c r="C40" s="26" t="s">
-        <v>67</v>
-      </c>
-      <c r="D40" s="26" t="s">
-        <v>68</v>
-      </c>
-      <c r="E40" s="26" t="s">
-        <v>69</v>
-      </c>
-      <c r="F40" s="26" t="s">
-        <v>70</v>
+      <c r="A40" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B40" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C40" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D40" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E40" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="F40" s="28" t="s">
+        <v>78</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3449,12 +3514,18 @@
       <c r="B41" s="29" t="s">
         <v>13</v>
       </c>
-      <c r="C41" s="16"/>
-      <c r="D41" s="11"/>
+      <c r="C41" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="D41" s="11" t="n">
+        <v>0.9</v>
+      </c>
       <c r="E41" s="12" t="n">
         <v>3</v>
       </c>
-      <c r="F41" s="12"/>
+      <c r="F41" s="12" t="n">
+        <v>4.5</v>
+      </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="12" t="n">
@@ -3463,64 +3534,198 @@
       <c r="B42" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="C42" s="17"/>
-      <c r="D42" s="18"/>
+      <c r="C42" s="17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D42" s="18" t="n">
+        <v>0</v>
+      </c>
       <c r="E42" s="19" t="n">
         <v>3</v>
       </c>
-      <c r="F42" s="19"/>
+      <c r="F42" s="19" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="12" t="n">
         <v>3</v>
       </c>
       <c r="B43" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C43" s="17" t="s">
         <v>50</v>
       </c>
-      <c r="C43" s="17"/>
-      <c r="D43" s="18"/>
+      <c r="D43" s="18" t="n">
+        <v>0</v>
+      </c>
       <c r="E43" s="19" t="n">
         <v>0.5</v>
       </c>
-      <c r="F43" s="32"/>
+      <c r="F43" s="32" t="n">
+        <v>0</v>
+      </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="12" t="n">
         <v>4</v>
       </c>
       <c r="B44" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="C44" s="17"/>
-      <c r="D44" s="18"/>
+        <v>52</v>
+      </c>
+      <c r="C44" s="17" t="s">
+        <v>52</v>
+      </c>
+      <c r="D44" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="E44" s="33" t="n">
         <v>0.5</v>
       </c>
-      <c r="F44" s="19"/>
+      <c r="F44" s="19" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="12" t="n">
         <v>5</v>
       </c>
       <c r="B45" s="20" t="s">
-        <v>52</v>
-      </c>
-      <c r="C45" s="17"/>
-      <c r="D45" s="18"/>
+        <v>53</v>
+      </c>
+      <c r="C45" s="17" t="s">
+        <v>53</v>
+      </c>
+      <c r="D45" s="18" t="n">
+        <v>1</v>
+      </c>
       <c r="E45" s="19" t="n">
         <v>1</v>
       </c>
-      <c r="F45" s="32"/>
+      <c r="F45" s="32" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="24"/>
-      <c r="C46" s="24"/>
-      <c r="E46" s="25" t="n">
+      <c r="B46" s="26"/>
+      <c r="C46" s="26"/>
+      <c r="E46" s="27" t="n">
         <f aca="false">SUM(E41:E45)</f>
         <v>8</v>
       </c>
-      <c r="F46" s="25" t="n">
+      <c r="F46" s="27" t="n">
         <f aca="false">SUM(F41:F45)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="28" t="s">
+        <v>2</v>
+      </c>
+      <c r="B49" s="28" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="D49" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="E49" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="F49" s="28" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="B50" s="29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C50" s="16"/>
+      <c r="D50" s="11"/>
+      <c r="E50" s="12" t="n">
+        <v>1</v>
+      </c>
+      <c r="F50" s="12"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="12" t="n">
+        <v>2</v>
+      </c>
+      <c r="B51" s="29" t="s">
+        <v>16</v>
+      </c>
+      <c r="C51" s="17"/>
+      <c r="D51" s="18"/>
+      <c r="E51" s="19" t="n">
+        <v>5</v>
+      </c>
+      <c r="F51" s="19"/>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="12" t="n">
+        <v>3</v>
+      </c>
+      <c r="B52" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="C52" s="17"/>
+      <c r="D52" s="18"/>
+      <c r="E52" s="19" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F52" s="32"/>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="12" t="n">
+        <v>4</v>
+      </c>
+      <c r="B53" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="C53" s="17"/>
+      <c r="D53" s="18"/>
+      <c r="E53" s="33" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F53" s="19"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="12" t="n">
+        <v>5</v>
+      </c>
+      <c r="B54" s="20" t="s">
+        <v>53</v>
+      </c>
+      <c r="C54" s="17"/>
+      <c r="D54" s="18"/>
+      <c r="E54" s="19" t="n">
+        <v>1</v>
+      </c>
+      <c r="F54" s="32"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B55" s="26"/>
+      <c r="C55" s="26"/>
+      <c r="E55" s="27" t="n">
+        <f aca="false">SUM(E50:E54)</f>
+        <v>8</v>
+      </c>
+      <c r="F55" s="27" t="n">
+        <f aca="false">SUM(F50:F54)</f>
         <v>0</v>
       </c>
     </row>
@@ -3548,34 +3753,32 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="8.36734693877551"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="54.5357142857143"/>
-    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="53.1887755102041"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="34" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="57.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="13" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="46.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="35" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="23.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="35" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>

</xml_diff>